<commit_message>
update mortality to include all years
</commit_message>
<xml_diff>
--- a/data_clean/mortality_cocaine_fentanyl.xlsx
+++ b/data_clean/mortality_cocaine_fentanyl.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -394,19 +394,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C2">
-        <v>878</v>
+        <v>220</v>
       </c>
       <c r="D2">
-        <v>692</v>
+        <v>473</v>
       </c>
       <c r="E2">
-        <v>514</v>
+        <v>461</v>
       </c>
       <c r="F2">
-        <v>1056</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3">
@@ -414,19 +414,19 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C3">
-        <v>1463</v>
+        <v>223</v>
       </c>
       <c r="D3">
-        <v>1054</v>
+        <v>394</v>
       </c>
       <c r="E3">
-        <v>595</v>
+        <v>376</v>
       </c>
       <c r="F3">
-        <v>1922</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4">
@@ -434,19 +434,19 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C4">
-        <v>1557</v>
+        <v>198</v>
       </c>
       <c r="D4">
-        <v>1059</v>
+        <v>404</v>
       </c>
       <c r="E4">
-        <v>587</v>
+        <v>396</v>
       </c>
       <c r="F4">
-        <v>2029</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5">
@@ -454,19 +454,19 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C5">
-        <v>1703</v>
+        <v>229</v>
       </c>
       <c r="D5">
-        <v>1103</v>
+        <v>410</v>
       </c>
       <c r="E5">
-        <v>602</v>
+        <v>389</v>
       </c>
       <c r="F5">
-        <v>2204</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6">
@@ -474,19 +474,19 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C6">
-        <v>1140</v>
+        <v>210</v>
       </c>
       <c r="D6">
-        <v>792</v>
+        <v>434</v>
       </c>
       <c r="E6">
-        <v>528</v>
+        <v>423</v>
       </c>
       <c r="F6">
-        <v>1404</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
@@ -494,19 +494,19 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C7">
-        <v>1261</v>
+        <v>193</v>
       </c>
       <c r="D7">
-        <v>913</v>
+        <v>511</v>
       </c>
       <c r="E7">
-        <v>616</v>
+        <v>490</v>
       </c>
       <c r="F7">
-        <v>1558</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
@@ -514,19 +514,19 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C8">
-        <v>1238</v>
+        <v>209</v>
       </c>
       <c r="D8">
-        <v>875</v>
+        <v>475</v>
       </c>
       <c r="E8">
-        <v>547</v>
+        <v>459</v>
       </c>
       <c r="F8">
-        <v>1566</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9">
@@ -534,19 +534,19 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C9">
-        <v>1276</v>
+        <v>211</v>
       </c>
       <c r="D9">
-        <v>855</v>
+        <v>434</v>
       </c>
       <c r="E9">
-        <v>556</v>
+        <v>415</v>
       </c>
       <c r="F9">
-        <v>1575</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10">
@@ -554,19 +554,19 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C10">
-        <v>1191</v>
+        <v>199</v>
       </c>
       <c r="D10">
-        <v>840</v>
+        <v>409</v>
       </c>
       <c r="E10">
-        <v>541</v>
+        <v>388</v>
       </c>
       <c r="F10">
-        <v>1490</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11">
@@ -574,19 +574,19 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C11">
-        <v>1282</v>
+        <v>234</v>
       </c>
       <c r="D11">
-        <v>1062</v>
+        <v>358</v>
       </c>
       <c r="E11">
-        <v>701</v>
+        <v>346</v>
       </c>
       <c r="F11">
-        <v>1643</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12">
@@ -594,19 +594,19 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C12">
-        <v>1232</v>
+        <v>232</v>
       </c>
       <c r="D12">
-        <v>1020</v>
+        <v>374</v>
       </c>
       <c r="E12">
-        <v>642</v>
+        <v>356</v>
       </c>
       <c r="F12">
-        <v>1610</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13">
@@ -614,19 +614,19 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C13">
-        <v>1325</v>
+        <v>196</v>
       </c>
       <c r="D13">
-        <v>1029</v>
+        <v>354</v>
       </c>
       <c r="E13">
-        <v>605</v>
+        <v>345</v>
       </c>
       <c r="F13">
-        <v>1749</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
@@ -634,19 +634,19 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C14">
-        <v>1942</v>
+        <v>251</v>
       </c>
       <c r="D14">
-        <v>1203</v>
+        <v>378</v>
       </c>
       <c r="E14">
-        <v>648</v>
+        <v>364</v>
       </c>
       <c r="F14">
-        <v>2497</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15">
@@ -654,19 +654,19 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C15">
-        <v>1826</v>
+        <v>249</v>
       </c>
       <c r="D15">
-        <v>1225</v>
+        <v>460</v>
       </c>
       <c r="E15">
-        <v>599</v>
+        <v>438</v>
       </c>
       <c r="F15">
-        <v>2452</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16">
@@ -674,19 +674,19 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C16">
-        <v>1782</v>
+        <v>269</v>
       </c>
       <c r="D16">
-        <v>1197</v>
+        <v>459</v>
       </c>
       <c r="E16">
-        <v>543</v>
+        <v>431</v>
       </c>
       <c r="F16">
-        <v>2436</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17">
@@ -694,19 +694,19 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C17">
-        <v>1888</v>
+        <v>366</v>
       </c>
       <c r="D17">
-        <v>1319</v>
+        <v>482</v>
       </c>
       <c r="E17">
-        <v>623</v>
+        <v>444</v>
       </c>
       <c r="F17">
-        <v>2584</v>
+        <v>404</v>
       </c>
     </row>
     <row r="18">
@@ -714,19 +714,19 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C18">
-        <v>1809</v>
+        <v>227</v>
       </c>
       <c r="D18">
-        <v>1134</v>
+        <v>445</v>
       </c>
       <c r="E18">
-        <v>615</v>
+        <v>428</v>
       </c>
       <c r="F18">
-        <v>2328</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19">
@@ -734,19 +734,19 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C19">
-        <v>1804</v>
+        <v>226</v>
       </c>
       <c r="D19">
-        <v>1271</v>
+        <v>501</v>
       </c>
       <c r="E19">
-        <v>680</v>
+        <v>478</v>
       </c>
       <c r="F19">
-        <v>2395</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20">
@@ -754,19 +754,19 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C20">
-        <v>1668</v>
+        <v>230</v>
       </c>
       <c r="D20">
-        <v>1299</v>
+        <v>487</v>
       </c>
       <c r="E20">
-        <v>691</v>
+        <v>466</v>
       </c>
       <c r="F20">
-        <v>2276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21">
@@ -774,19 +774,19 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C21">
-        <v>1789</v>
+        <v>263</v>
       </c>
       <c r="D21">
-        <v>1242</v>
+        <v>482</v>
       </c>
       <c r="E21">
-        <v>648</v>
+        <v>459</v>
       </c>
       <c r="F21">
-        <v>2383</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22">
@@ -794,19 +794,19 @@
         <v>6</v>
       </c>
       <c r="B22">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C22">
-        <v>1789</v>
+        <v>245</v>
       </c>
       <c r="D22">
-        <v>1286</v>
+        <v>488</v>
       </c>
       <c r="E22">
-        <v>684</v>
+        <v>473</v>
       </c>
       <c r="F22">
-        <v>2391</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23">
@@ -814,19 +814,19 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C23">
-        <v>1755</v>
+        <v>213</v>
       </c>
       <c r="D23">
-        <v>1249</v>
+        <v>490</v>
       </c>
       <c r="E23">
-        <v>672</v>
+        <v>472</v>
       </c>
       <c r="F23">
-        <v>2332</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24">
@@ -834,19 +834,19 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C24">
-        <v>1781</v>
+        <v>209</v>
       </c>
       <c r="D24">
-        <v>1332</v>
+        <v>438</v>
       </c>
       <c r="E24">
-        <v>661</v>
+        <v>425</v>
       </c>
       <c r="F24">
-        <v>2452</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25">
@@ -854,19 +854,19 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="C25">
-        <v>1859</v>
+        <v>228</v>
       </c>
       <c r="D25">
-        <v>1265</v>
+        <v>422</v>
       </c>
       <c r="E25">
-        <v>585</v>
+        <v>406</v>
       </c>
       <c r="F25">
-        <v>2539</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26">
@@ -874,19 +874,19 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C26">
-        <v>1896</v>
+        <v>467</v>
       </c>
       <c r="D26">
-        <v>1282</v>
+        <v>477</v>
       </c>
       <c r="E26">
-        <v>600</v>
+        <v>427</v>
       </c>
       <c r="F26">
-        <v>2578</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27">
@@ -894,19 +894,19 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C27">
-        <v>2008</v>
+        <v>500</v>
       </c>
       <c r="D27">
-        <v>1280</v>
+        <v>514</v>
       </c>
       <c r="E27">
+        <v>450</v>
+      </c>
+      <c r="F27">
         <v>564</v>
-      </c>
-      <c r="F27">
-        <v>2724</v>
       </c>
     </row>
     <row r="28">
@@ -914,19 +914,19 @@
         <v>11</v>
       </c>
       <c r="B28">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C28">
-        <v>1926</v>
+        <v>514</v>
       </c>
       <c r="D28">
-        <v>1163</v>
+        <v>506</v>
       </c>
       <c r="E28">
-        <v>490</v>
+        <v>441</v>
       </c>
       <c r="F28">
-        <v>2599</v>
+        <v>579</v>
       </c>
     </row>
     <row r="29">
@@ -934,19 +934,19 @@
         <v>12</v>
       </c>
       <c r="B29">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C29">
-        <v>1993</v>
+        <v>570</v>
       </c>
       <c r="D29">
-        <v>1233</v>
+        <v>542</v>
       </c>
       <c r="E29">
-        <v>531</v>
+        <v>466</v>
       </c>
       <c r="F29">
-        <v>2695</v>
+        <v>646</v>
       </c>
     </row>
     <row r="30">
@@ -954,19 +954,19 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C30">
-        <v>1747</v>
+        <v>383</v>
       </c>
       <c r="D30">
-        <v>1204</v>
+        <v>511</v>
       </c>
       <c r="E30">
-        <v>548</v>
+        <v>458</v>
       </c>
       <c r="F30">
-        <v>2403</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31">
@@ -974,19 +974,19 @@
         <v>3</v>
       </c>
       <c r="B31">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C31">
-        <v>1951</v>
+        <v>418</v>
       </c>
       <c r="D31">
-        <v>1406</v>
+        <v>546</v>
       </c>
       <c r="E31">
-        <v>636</v>
+        <v>491</v>
       </c>
       <c r="F31">
-        <v>2721</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32">
@@ -994,19 +994,19 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C32">
-        <v>1876</v>
+        <v>340</v>
       </c>
       <c r="D32">
-        <v>1365</v>
+        <v>446</v>
       </c>
       <c r="E32">
-        <v>616</v>
+        <v>409</v>
       </c>
       <c r="F32">
-        <v>2625</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33">
@@ -1014,19 +1014,19 @@
         <v>5</v>
       </c>
       <c r="B33">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C33">
-        <v>1911</v>
+        <v>365</v>
       </c>
       <c r="D33">
-        <v>1423</v>
+        <v>519</v>
       </c>
       <c r="E33">
-        <v>622</v>
+        <v>465</v>
       </c>
       <c r="F33">
-        <v>2712</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34">
@@ -1034,19 +1034,19 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C34">
-        <v>1963</v>
+        <v>376</v>
       </c>
       <c r="D34">
-        <v>1421</v>
+        <v>503</v>
       </c>
       <c r="E34">
-        <v>611</v>
+        <v>459</v>
       </c>
       <c r="F34">
-        <v>2773</v>
+        <v>420</v>
       </c>
     </row>
     <row r="35">
@@ -1054,19 +1054,19 @@
         <v>7</v>
       </c>
       <c r="B35">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C35">
-        <v>1962</v>
+        <v>392</v>
       </c>
       <c r="D35">
-        <v>1375</v>
+        <v>496</v>
       </c>
       <c r="E35">
-        <v>574</v>
+        <v>461</v>
       </c>
       <c r="F35">
-        <v>2763</v>
+        <v>427</v>
       </c>
     </row>
     <row r="36">
@@ -1074,19 +1074,19 @@
         <v>8</v>
       </c>
       <c r="B36">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C36">
-        <v>1995</v>
+        <v>381</v>
       </c>
       <c r="D36">
-        <v>1353</v>
+        <v>502</v>
       </c>
       <c r="E36">
-        <v>593</v>
+        <v>462</v>
       </c>
       <c r="F36">
-        <v>2755</v>
+        <v>421</v>
       </c>
     </row>
     <row r="37">
@@ -1094,19 +1094,19 @@
         <v>9</v>
       </c>
       <c r="B37">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C37">
-        <v>1951</v>
+        <v>369</v>
       </c>
       <c r="D37">
-        <v>1257</v>
+        <v>464</v>
       </c>
       <c r="E37">
-        <v>551</v>
+        <v>400</v>
       </c>
       <c r="F37">
-        <v>2657</v>
+        <v>433</v>
       </c>
     </row>
     <row r="38">
@@ -1114,19 +1114,19 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C38">
-        <v>1965</v>
+        <v>612</v>
       </c>
       <c r="D38">
-        <v>1229</v>
+        <v>544</v>
       </c>
       <c r="E38">
-        <v>545</v>
+        <v>433</v>
       </c>
       <c r="F38">
-        <v>2649</v>
+        <v>723</v>
       </c>
     </row>
     <row r="39">
@@ -1134,19 +1134,19 @@
         <v>10</v>
       </c>
       <c r="B39">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C39">
-        <v>2454</v>
+        <v>840</v>
       </c>
       <c r="D39">
-        <v>1569</v>
+        <v>669</v>
       </c>
       <c r="E39">
-        <v>579</v>
+        <v>502</v>
       </c>
       <c r="F39">
-        <v>3444</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="40">
@@ -1154,19 +1154,19 @@
         <v>11</v>
       </c>
       <c r="B40">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C40">
-        <v>2544</v>
+        <v>706</v>
       </c>
       <c r="D40">
-        <v>1561</v>
+        <v>628</v>
       </c>
       <c r="E40">
-        <v>574</v>
+        <v>471</v>
       </c>
       <c r="F40">
-        <v>3531</v>
+        <v>863</v>
       </c>
     </row>
     <row r="41">
@@ -1174,19 +1174,19 @@
         <v>12</v>
       </c>
       <c r="B41">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C41">
-        <v>2630</v>
+        <v>715</v>
       </c>
       <c r="D41">
-        <v>1554</v>
+        <v>659</v>
       </c>
       <c r="E41">
-        <v>550</v>
+        <v>508</v>
       </c>
       <c r="F41">
-        <v>3634</v>
+        <v>866</v>
       </c>
     </row>
     <row r="42">
@@ -1194,19 +1194,19 @@
         <v>2</v>
       </c>
       <c r="B42">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C42">
-        <v>1864</v>
+        <v>627</v>
       </c>
       <c r="D42">
-        <v>1197</v>
+        <v>610</v>
       </c>
       <c r="E42">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="F42">
-        <v>2565</v>
+        <v>752</v>
       </c>
     </row>
     <row r="43">
@@ -1214,19 +1214,19 @@
         <v>3</v>
       </c>
       <c r="B43">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C43">
-        <v>2212</v>
+        <v>663</v>
       </c>
       <c r="D43">
-        <v>1362</v>
+        <v>693</v>
       </c>
       <c r="E43">
-        <v>591</v>
+        <v>563</v>
       </c>
       <c r="F43">
-        <v>2983</v>
+        <v>793</v>
       </c>
     </row>
     <row r="44">
@@ -1234,19 +1234,19 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C44">
-        <v>1991</v>
+        <v>731</v>
       </c>
       <c r="D44">
-        <v>1335</v>
+        <v>615</v>
       </c>
       <c r="E44">
-        <v>536</v>
+        <v>474</v>
       </c>
       <c r="F44">
-        <v>2790</v>
+        <v>872</v>
       </c>
     </row>
     <row r="45">
@@ -1254,19 +1254,19 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C45">
-        <v>2092</v>
+        <v>695</v>
       </c>
       <c r="D45">
-        <v>1422</v>
+        <v>605</v>
       </c>
       <c r="E45">
-        <v>614</v>
+        <v>486</v>
       </c>
       <c r="F45">
-        <v>2900</v>
+        <v>814</v>
       </c>
     </row>
     <row r="46">
@@ -1274,19 +1274,19 @@
         <v>6</v>
       </c>
       <c r="B46">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C46">
-        <v>2111</v>
+        <v>633</v>
       </c>
       <c r="D46">
-        <v>1401</v>
+        <v>548</v>
       </c>
       <c r="E46">
-        <v>531</v>
+        <v>452</v>
       </c>
       <c r="F46">
-        <v>2981</v>
+        <v>729</v>
       </c>
     </row>
     <row r="47">
@@ -1294,19 +1294,19 @@
         <v>7</v>
       </c>
       <c r="B47">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C47">
-        <v>2329</v>
+        <v>655</v>
       </c>
       <c r="D47">
-        <v>1478</v>
+        <v>637</v>
       </c>
       <c r="E47">
-        <v>602</v>
+        <v>529</v>
       </c>
       <c r="F47">
-        <v>3205</v>
+        <v>763</v>
       </c>
     </row>
     <row r="48">
@@ -1314,19 +1314,19 @@
         <v>8</v>
       </c>
       <c r="B48">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C48">
-        <v>2308</v>
+        <v>646</v>
       </c>
       <c r="D48">
-        <v>1529</v>
+        <v>641</v>
       </c>
       <c r="E48">
-        <v>590</v>
+        <v>527</v>
       </c>
       <c r="F48">
-        <v>3247</v>
+        <v>760</v>
       </c>
     </row>
     <row r="49">
@@ -1334,19 +1334,19 @@
         <v>9</v>
       </c>
       <c r="B49">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="C49">
-        <v>2286</v>
+        <v>744</v>
       </c>
       <c r="D49">
-        <v>1434</v>
+        <v>618</v>
       </c>
       <c r="E49">
-        <v>520</v>
+        <v>471</v>
       </c>
       <c r="F49">
-        <v>3200</v>
+        <v>891</v>
       </c>
     </row>
     <row r="50">
@@ -1354,19 +1354,19 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C50">
-        <v>2668</v>
+        <v>878</v>
       </c>
       <c r="D50">
-        <v>1583</v>
+        <v>692</v>
       </c>
       <c r="E50">
-        <v>607</v>
+        <v>514</v>
       </c>
       <c r="F50">
-        <v>3644</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="51">
@@ -1374,19 +1374,19 @@
         <v>10</v>
       </c>
       <c r="B51">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C51">
-        <v>3621</v>
+        <v>1463</v>
       </c>
       <c r="D51">
-        <v>1548</v>
+        <v>1054</v>
       </c>
       <c r="E51">
-        <v>464</v>
+        <v>595</v>
       </c>
       <c r="F51">
-        <v>4705</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="52">
@@ -1394,19 +1394,19 @@
         <v>11</v>
       </c>
       <c r="B52">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C52">
-        <v>3703</v>
+        <v>1557</v>
       </c>
       <c r="D52">
-        <v>1468</v>
+        <v>1059</v>
       </c>
       <c r="E52">
-        <v>433</v>
+        <v>587</v>
       </c>
       <c r="F52">
-        <v>4738</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="53">
@@ -1414,19 +1414,19 @@
         <v>12</v>
       </c>
       <c r="B53">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C53">
-        <v>3824</v>
+        <v>1703</v>
       </c>
       <c r="D53">
-        <v>1524</v>
+        <v>1103</v>
       </c>
       <c r="E53">
-        <v>456</v>
+        <v>602</v>
       </c>
       <c r="F53">
-        <v>4892</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="54">
@@ -1434,19 +1434,19 @@
         <v>2</v>
       </c>
       <c r="B54">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C54">
-        <v>2684</v>
+        <v>1140</v>
       </c>
       <c r="D54">
-        <v>1610</v>
+        <v>792</v>
       </c>
       <c r="E54">
-        <v>556</v>
+        <v>528</v>
       </c>
       <c r="F54">
-        <v>3738</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="55">
@@ -1454,19 +1454,19 @@
         <v>3</v>
       </c>
       <c r="B55">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C55">
-        <v>3053</v>
+        <v>1261</v>
       </c>
       <c r="D55">
-        <v>1859</v>
+        <v>913</v>
       </c>
       <c r="E55">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="F55">
-        <v>4299</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="56">
@@ -1474,19 +1474,19 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C56">
-        <v>3579</v>
+        <v>1238</v>
       </c>
       <c r="D56">
-        <v>2015</v>
+        <v>875</v>
       </c>
       <c r="E56">
-        <v>637</v>
+        <v>547</v>
       </c>
       <c r="F56">
-        <v>4957</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="57">
@@ -1494,19 +1494,19 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C57">
-        <v>4653</v>
+        <v>1276</v>
       </c>
       <c r="D57">
-        <v>2222</v>
+        <v>855</v>
       </c>
       <c r="E57">
-        <v>628</v>
+        <v>556</v>
       </c>
       <c r="F57">
-        <v>6247</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="58">
@@ -1514,19 +1514,19 @@
         <v>6</v>
       </c>
       <c r="B58">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C58">
-        <v>4060</v>
+        <v>1191</v>
       </c>
       <c r="D58">
-        <v>1825</v>
+        <v>840</v>
       </c>
       <c r="E58">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="F58">
-        <v>5337</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="59">
@@ -1534,19 +1534,19 @@
         <v>7</v>
       </c>
       <c r="B59">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C59">
-        <v>4101</v>
+        <v>1282</v>
       </c>
       <c r="D59">
-        <v>1743</v>
+        <v>1062</v>
       </c>
       <c r="E59">
-        <v>560</v>
+        <v>701</v>
       </c>
       <c r="F59">
-        <v>5284</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="60">
@@ -1554,19 +1554,19 @@
         <v>8</v>
       </c>
       <c r="B60">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C60">
-        <v>3976</v>
+        <v>1232</v>
       </c>
       <c r="D60">
-        <v>1673</v>
+        <v>1020</v>
       </c>
       <c r="E60">
-        <v>522</v>
+        <v>642</v>
       </c>
       <c r="F60">
-        <v>5127</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="61">
@@ -1574,19 +1574,19 @@
         <v>9</v>
       </c>
       <c r="B61">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="C61">
-        <v>3689</v>
+        <v>1325</v>
       </c>
       <c r="D61">
-        <v>1618</v>
+        <v>1029</v>
       </c>
       <c r="E61">
-        <v>498</v>
+        <v>605</v>
       </c>
       <c r="F61">
-        <v>4809</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="62">
@@ -1594,19 +1594,19 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C62">
-        <v>4333</v>
+        <v>1942</v>
       </c>
       <c r="D62">
-        <v>1937</v>
+        <v>1203</v>
       </c>
       <c r="E62">
-        <v>584</v>
+        <v>648</v>
       </c>
       <c r="F62">
-        <v>5686</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="63">
@@ -1614,19 +1614,19 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C63">
-        <v>4447</v>
+        <v>1826</v>
       </c>
       <c r="D63">
-        <v>2232</v>
+        <v>1225</v>
       </c>
       <c r="E63">
-        <v>625</v>
+        <v>599</v>
       </c>
       <c r="F63">
-        <v>6054</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="64">
@@ -1634,19 +1634,19 @@
         <v>11</v>
       </c>
       <c r="B64">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C64">
-        <v>4202</v>
+        <v>1782</v>
       </c>
       <c r="D64">
-        <v>2125</v>
+        <v>1197</v>
       </c>
       <c r="E64">
-        <v>582</v>
+        <v>543</v>
       </c>
       <c r="F64">
-        <v>5745</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="65">
@@ -1654,19 +1654,19 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C65">
-        <v>4419</v>
+        <v>1888</v>
       </c>
       <c r="D65">
-        <v>2226</v>
+        <v>1319</v>
       </c>
       <c r="E65">
-        <v>646</v>
+        <v>623</v>
       </c>
       <c r="F65">
-        <v>5999</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="66">
@@ -1674,19 +1674,19 @@
         <v>2</v>
       </c>
       <c r="B66">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C66">
-        <v>3813</v>
+        <v>1809</v>
       </c>
       <c r="D66">
-        <v>1698</v>
+        <v>1134</v>
       </c>
       <c r="E66">
-        <v>503</v>
+        <v>615</v>
       </c>
       <c r="F66">
-        <v>5008</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="67">
@@ -1694,19 +1694,19 @@
         <v>3</v>
       </c>
       <c r="B67">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C67">
-        <v>4775</v>
+        <v>1804</v>
       </c>
       <c r="D67">
-        <v>2211</v>
+        <v>1271</v>
       </c>
       <c r="E67">
-        <v>621</v>
+        <v>680</v>
       </c>
       <c r="F67">
-        <v>6365</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="68">
@@ -1714,19 +1714,19 @@
         <v>4</v>
       </c>
       <c r="B68">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C68">
-        <v>4721</v>
+        <v>1668</v>
       </c>
       <c r="D68">
-        <v>2361</v>
+        <v>1299</v>
       </c>
       <c r="E68">
-        <v>684</v>
+        <v>691</v>
       </c>
       <c r="F68">
-        <v>6398</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="69">
@@ -1734,19 +1734,19 @@
         <v>5</v>
       </c>
       <c r="B69">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C69">
-        <v>4671</v>
+        <v>1789</v>
       </c>
       <c r="D69">
-        <v>2241</v>
+        <v>1242</v>
       </c>
       <c r="E69">
-        <v>620</v>
+        <v>648</v>
       </c>
       <c r="F69">
-        <v>6292</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="70">
@@ -1754,19 +1754,19 @@
         <v>6</v>
       </c>
       <c r="B70">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C70">
-        <v>4562</v>
+        <v>1789</v>
       </c>
       <c r="D70">
-        <v>2149</v>
+        <v>1286</v>
       </c>
       <c r="E70">
-        <v>642</v>
+        <v>684</v>
       </c>
       <c r="F70">
-        <v>6069</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="71">
@@ -1774,19 +1774,19 @@
         <v>7</v>
       </c>
       <c r="B71">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C71">
-        <v>4631</v>
+        <v>1755</v>
       </c>
       <c r="D71">
-        <v>2254</v>
+        <v>1249</v>
       </c>
       <c r="E71">
-        <v>665</v>
+        <v>672</v>
       </c>
       <c r="F71">
-        <v>6220</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="72">
@@ -1794,19 +1794,19 @@
         <v>8</v>
       </c>
       <c r="B72">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C72">
-        <v>4669</v>
+        <v>1781</v>
       </c>
       <c r="D72">
-        <v>2312</v>
+        <v>1332</v>
       </c>
       <c r="E72">
-        <v>692</v>
+        <v>661</v>
       </c>
       <c r="F72">
-        <v>6289</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="73">
@@ -1814,18 +1814,978 @@
         <v>9</v>
       </c>
       <c r="B73">
+        <v>2017</v>
+      </c>
+      <c r="C73">
+        <v>1859</v>
+      </c>
+      <c r="D73">
+        <v>1265</v>
+      </c>
+      <c r="E73">
+        <v>585</v>
+      </c>
+      <c r="F73">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>2018</v>
+      </c>
+      <c r="C74">
+        <v>1896</v>
+      </c>
+      <c r="D74">
+        <v>1282</v>
+      </c>
+      <c r="E74">
+        <v>600</v>
+      </c>
+      <c r="F74">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>2018</v>
+      </c>
+      <c r="C75">
+        <v>2008</v>
+      </c>
+      <c r="D75">
+        <v>1280</v>
+      </c>
+      <c r="E75">
+        <v>564</v>
+      </c>
+      <c r="F75">
+        <v>2724</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>2018</v>
+      </c>
+      <c r="C76">
+        <v>1926</v>
+      </c>
+      <c r="D76">
+        <v>1163</v>
+      </c>
+      <c r="E76">
+        <v>490</v>
+      </c>
+      <c r="F76">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>12</v>
+      </c>
+      <c r="B77">
+        <v>2018</v>
+      </c>
+      <c r="C77">
+        <v>1993</v>
+      </c>
+      <c r="D77">
+        <v>1233</v>
+      </c>
+      <c r="E77">
+        <v>531</v>
+      </c>
+      <c r="F77">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78">
+        <v>2018</v>
+      </c>
+      <c r="C78">
+        <v>1747</v>
+      </c>
+      <c r="D78">
+        <v>1204</v>
+      </c>
+      <c r="E78">
+        <v>548</v>
+      </c>
+      <c r="F78">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>2018</v>
+      </c>
+      <c r="C79">
+        <v>1951</v>
+      </c>
+      <c r="D79">
+        <v>1406</v>
+      </c>
+      <c r="E79">
+        <v>636</v>
+      </c>
+      <c r="F79">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>2018</v>
+      </c>
+      <c r="C80">
+        <v>1876</v>
+      </c>
+      <c r="D80">
+        <v>1365</v>
+      </c>
+      <c r="E80">
+        <v>616</v>
+      </c>
+      <c r="F80">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>2018</v>
+      </c>
+      <c r="C81">
+        <v>1911</v>
+      </c>
+      <c r="D81">
+        <v>1423</v>
+      </c>
+      <c r="E81">
+        <v>622</v>
+      </c>
+      <c r="F81">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>6</v>
+      </c>
+      <c r="B82">
+        <v>2018</v>
+      </c>
+      <c r="C82">
+        <v>1963</v>
+      </c>
+      <c r="D82">
+        <v>1421</v>
+      </c>
+      <c r="E82">
+        <v>611</v>
+      </c>
+      <c r="F82">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="B83">
+        <v>2018</v>
+      </c>
+      <c r="C83">
+        <v>1962</v>
+      </c>
+      <c r="D83">
+        <v>1375</v>
+      </c>
+      <c r="E83">
+        <v>574</v>
+      </c>
+      <c r="F83">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>8</v>
+      </c>
+      <c r="B84">
+        <v>2018</v>
+      </c>
+      <c r="C84">
+        <v>1995</v>
+      </c>
+      <c r="D84">
+        <v>1353</v>
+      </c>
+      <c r="E84">
+        <v>593</v>
+      </c>
+      <c r="F84">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>9</v>
+      </c>
+      <c r="B85">
+        <v>2018</v>
+      </c>
+      <c r="C85">
+        <v>1951</v>
+      </c>
+      <c r="D85">
+        <v>1257</v>
+      </c>
+      <c r="E85">
+        <v>551</v>
+      </c>
+      <c r="F85">
+        <v>2657</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>2019</v>
+      </c>
+      <c r="C86">
+        <v>1965</v>
+      </c>
+      <c r="D86">
+        <v>1229</v>
+      </c>
+      <c r="E86">
+        <v>545</v>
+      </c>
+      <c r="F86">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87">
+        <v>2019</v>
+      </c>
+      <c r="C87">
+        <v>2454</v>
+      </c>
+      <c r="D87">
+        <v>1569</v>
+      </c>
+      <c r="E87">
+        <v>579</v>
+      </c>
+      <c r="F87">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>11</v>
+      </c>
+      <c r="B88">
+        <v>2019</v>
+      </c>
+      <c r="C88">
+        <v>2544</v>
+      </c>
+      <c r="D88">
+        <v>1561</v>
+      </c>
+      <c r="E88">
+        <v>574</v>
+      </c>
+      <c r="F88">
+        <v>3531</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>12</v>
+      </c>
+      <c r="B89">
+        <v>2019</v>
+      </c>
+      <c r="C89">
+        <v>2630</v>
+      </c>
+      <c r="D89">
+        <v>1554</v>
+      </c>
+      <c r="E89">
+        <v>550</v>
+      </c>
+      <c r="F89">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>2019</v>
+      </c>
+      <c r="C90">
+        <v>1864</v>
+      </c>
+      <c r="D90">
+        <v>1197</v>
+      </c>
+      <c r="E90">
+        <v>496</v>
+      </c>
+      <c r="F90">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>2019</v>
+      </c>
+      <c r="C91">
+        <v>2212</v>
+      </c>
+      <c r="D91">
+        <v>1362</v>
+      </c>
+      <c r="E91">
+        <v>591</v>
+      </c>
+      <c r="F91">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>2019</v>
+      </c>
+      <c r="C92">
+        <v>1991</v>
+      </c>
+      <c r="D92">
+        <v>1335</v>
+      </c>
+      <c r="E92">
+        <v>536</v>
+      </c>
+      <c r="F92">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>2019</v>
+      </c>
+      <c r="C93">
+        <v>2092</v>
+      </c>
+      <c r="D93">
+        <v>1422</v>
+      </c>
+      <c r="E93">
+        <v>614</v>
+      </c>
+      <c r="F93">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>2019</v>
+      </c>
+      <c r="C94">
+        <v>2111</v>
+      </c>
+      <c r="D94">
+        <v>1401</v>
+      </c>
+      <c r="E94">
+        <v>531</v>
+      </c>
+      <c r="F94">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>2019</v>
+      </c>
+      <c r="C95">
+        <v>2329</v>
+      </c>
+      <c r="D95">
+        <v>1478</v>
+      </c>
+      <c r="E95">
+        <v>602</v>
+      </c>
+      <c r="F95">
+        <v>3205</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>8</v>
+      </c>
+      <c r="B96">
+        <v>2019</v>
+      </c>
+      <c r="C96">
+        <v>2308</v>
+      </c>
+      <c r="D96">
+        <v>1529</v>
+      </c>
+      <c r="E96">
+        <v>590</v>
+      </c>
+      <c r="F96">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>2019</v>
+      </c>
+      <c r="C97">
+        <v>2286</v>
+      </c>
+      <c r="D97">
+        <v>1434</v>
+      </c>
+      <c r="E97">
+        <v>520</v>
+      </c>
+      <c r="F97">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>2020</v>
+      </c>
+      <c r="C98">
+        <v>2668</v>
+      </c>
+      <c r="D98">
+        <v>1583</v>
+      </c>
+      <c r="E98">
+        <v>607</v>
+      </c>
+      <c r="F98">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99">
+        <v>2020</v>
+      </c>
+      <c r="C99">
+        <v>3621</v>
+      </c>
+      <c r="D99">
+        <v>1548</v>
+      </c>
+      <c r="E99">
+        <v>464</v>
+      </c>
+      <c r="F99">
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>11</v>
+      </c>
+      <c r="B100">
+        <v>2020</v>
+      </c>
+      <c r="C100">
+        <v>3703</v>
+      </c>
+      <c r="D100">
+        <v>1468</v>
+      </c>
+      <c r="E100">
+        <v>433</v>
+      </c>
+      <c r="F100">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>12</v>
+      </c>
+      <c r="B101">
+        <v>2020</v>
+      </c>
+      <c r="C101">
+        <v>3824</v>
+      </c>
+      <c r="D101">
+        <v>1524</v>
+      </c>
+      <c r="E101">
+        <v>456</v>
+      </c>
+      <c r="F101">
+        <v>4892</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>2020</v>
+      </c>
+      <c r="C102">
+        <v>2684</v>
+      </c>
+      <c r="D102">
+        <v>1610</v>
+      </c>
+      <c r="E102">
+        <v>556</v>
+      </c>
+      <c r="F102">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>2020</v>
+      </c>
+      <c r="C103">
+        <v>3053</v>
+      </c>
+      <c r="D103">
+        <v>1859</v>
+      </c>
+      <c r="E103">
+        <v>613</v>
+      </c>
+      <c r="F103">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>2020</v>
+      </c>
+      <c r="C104">
+        <v>3579</v>
+      </c>
+      <c r="D104">
+        <v>2015</v>
+      </c>
+      <c r="E104">
+        <v>637</v>
+      </c>
+      <c r="F104">
+        <v>4957</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>5</v>
+      </c>
+      <c r="B105">
+        <v>2020</v>
+      </c>
+      <c r="C105">
+        <v>4653</v>
+      </c>
+      <c r="D105">
+        <v>2222</v>
+      </c>
+      <c r="E105">
+        <v>628</v>
+      </c>
+      <c r="F105">
+        <v>6247</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>6</v>
+      </c>
+      <c r="B106">
+        <v>2020</v>
+      </c>
+      <c r="C106">
+        <v>4060</v>
+      </c>
+      <c r="D106">
+        <v>1825</v>
+      </c>
+      <c r="E106">
+        <v>548</v>
+      </c>
+      <c r="F106">
+        <v>5337</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>7</v>
+      </c>
+      <c r="B107">
+        <v>2020</v>
+      </c>
+      <c r="C107">
+        <v>4101</v>
+      </c>
+      <c r="D107">
+        <v>1743</v>
+      </c>
+      <c r="E107">
+        <v>560</v>
+      </c>
+      <c r="F107">
+        <v>5284</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>8</v>
+      </c>
+      <c r="B108">
+        <v>2020</v>
+      </c>
+      <c r="C108">
+        <v>3976</v>
+      </c>
+      <c r="D108">
+        <v>1673</v>
+      </c>
+      <c r="E108">
+        <v>522</v>
+      </c>
+      <c r="F108">
+        <v>5127</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>9</v>
+      </c>
+      <c r="B109">
+        <v>2020</v>
+      </c>
+      <c r="C109">
+        <v>3689</v>
+      </c>
+      <c r="D109">
+        <v>1618</v>
+      </c>
+      <c r="E109">
+        <v>498</v>
+      </c>
+      <c r="F109">
+        <v>4809</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
         <v>2021</v>
       </c>
-      <c r="C73">
+      <c r="C110">
+        <v>4333</v>
+      </c>
+      <c r="D110">
+        <v>1937</v>
+      </c>
+      <c r="E110">
+        <v>584</v>
+      </c>
+      <c r="F110">
+        <v>5686</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>10</v>
+      </c>
+      <c r="B111">
+        <v>2021</v>
+      </c>
+      <c r="C111">
+        <v>4447</v>
+      </c>
+      <c r="D111">
+        <v>2232</v>
+      </c>
+      <c r="E111">
+        <v>625</v>
+      </c>
+      <c r="F111">
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>11</v>
+      </c>
+      <c r="B112">
+        <v>2021</v>
+      </c>
+      <c r="C112">
+        <v>4202</v>
+      </c>
+      <c r="D112">
+        <v>2125</v>
+      </c>
+      <c r="E112">
+        <v>582</v>
+      </c>
+      <c r="F112">
+        <v>5745</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>12</v>
+      </c>
+      <c r="B113">
+        <v>2021</v>
+      </c>
+      <c r="C113">
+        <v>4419</v>
+      </c>
+      <c r="D113">
+        <v>2226</v>
+      </c>
+      <c r="E113">
+        <v>646</v>
+      </c>
+      <c r="F113">
+        <v>5999</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>2021</v>
+      </c>
+      <c r="C114">
+        <v>3813</v>
+      </c>
+      <c r="D114">
+        <v>1698</v>
+      </c>
+      <c r="E114">
+        <v>503</v>
+      </c>
+      <c r="F114">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>2021</v>
+      </c>
+      <c r="C115">
+        <v>4775</v>
+      </c>
+      <c r="D115">
+        <v>2211</v>
+      </c>
+      <c r="E115">
+        <v>621</v>
+      </c>
+      <c r="F115">
+        <v>6365</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>4</v>
+      </c>
+      <c r="B116">
+        <v>2021</v>
+      </c>
+      <c r="C116">
+        <v>4721</v>
+      </c>
+      <c r="D116">
+        <v>2361</v>
+      </c>
+      <c r="E116">
+        <v>684</v>
+      </c>
+      <c r="F116">
+        <v>6398</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>2021</v>
+      </c>
+      <c r="C117">
+        <v>4671</v>
+      </c>
+      <c r="D117">
+        <v>2241</v>
+      </c>
+      <c r="E117">
+        <v>620</v>
+      </c>
+      <c r="F117">
+        <v>6292</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118">
+        <v>6</v>
+      </c>
+      <c r="B118">
+        <v>2021</v>
+      </c>
+      <c r="C118">
+        <v>4562</v>
+      </c>
+      <c r="D118">
+        <v>2149</v>
+      </c>
+      <c r="E118">
+        <v>642</v>
+      </c>
+      <c r="F118">
+        <v>6069</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>7</v>
+      </c>
+      <c r="B119">
+        <v>2021</v>
+      </c>
+      <c r="C119">
+        <v>4631</v>
+      </c>
+      <c r="D119">
+        <v>2254</v>
+      </c>
+      <c r="E119">
+        <v>665</v>
+      </c>
+      <c r="F119">
+        <v>6220</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>8</v>
+      </c>
+      <c r="B120">
+        <v>2021</v>
+      </c>
+      <c r="C120">
+        <v>4669</v>
+      </c>
+      <c r="D120">
+        <v>2312</v>
+      </c>
+      <c r="E120">
+        <v>692</v>
+      </c>
+      <c r="F120">
+        <v>6289</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121">
+        <v>9</v>
+      </c>
+      <c r="B121">
+        <v>2021</v>
+      </c>
+      <c r="C121">
         <v>4495</v>
       </c>
-      <c r="D73">
+      <c r="D121">
         <v>2218</v>
       </c>
-      <c r="E73">
+      <c r="E121">
         <v>601</v>
       </c>
-      <c r="F73">
+      <c r="F121">
         <v>6112</v>
       </c>
     </row>

</xml_diff>